<commit_message>
Email auf Unique gesetzt und Doku angepasst
</commit_message>
<xml_diff>
--- a/additional_files/db/Datenbank_Aufbau_Layout.xlsx
+++ b/additional_files/db/Datenbank_Aufbau_Layout.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5900" yWindow="1520" windowWidth="28800" windowHeight="15740"/>
+    <workbookView xWindow="5895" yWindow="1515" windowWidth="28800" windowHeight="15735"/>
   </bookViews>
   <sheets>
     <sheet name="Datenbank-Aufbau (Layout)" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="93">
   <si>
     <t>ID</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>Kunde (ID)</t>
+  </si>
+  <si>
+    <t>Unique</t>
   </si>
 </sst>
 </file>
@@ -962,14 +965,14 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="20" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -999,25 +1002,25 @@
     <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Besuchter Link" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="51" builtinId="9" hidden="1"/>
     <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Hinweis" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Link" xfId="42" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="44" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="46" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="48" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Titel" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
@@ -1323,27 +1326,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:K67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="2"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" style="2"/>
+    <col min="11" max="11" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>31</v>
       </c>
@@ -1354,36 +1359,40 @@
         <v>33</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="28"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="J1" s="28"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="10"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="J4" s="3" t="s">
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K4" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1393,14 +1402,14 @@
       <c r="C5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="25" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1410,11 +1419,11 @@
       <c r="C6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1424,11 +1433,11 @@
       <c r="C7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -1438,22 +1447,22 @@
       <c r="C8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1461,7 +1470,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1472,7 +1481,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1483,7 +1492,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>75</v>
       </c>
@@ -1494,29 +1503,29 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28">
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -1526,8 +1535,11 @@
       <c r="C16" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="D16" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -1537,11 +1549,11 @@
       <c r="C17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>73</v>
       </c>
@@ -1551,26 +1563,27 @@
       <c r="C18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="F18" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="3" customFormat="1">
+    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="5"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="5"/>
-      <c r="I20" s="28"/>
-    </row>
-    <row r="21" spans="1:9" ht="56">
+      <c r="H20" s="5"/>
+      <c r="J20" s="28"/>
+    </row>
+    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1580,17 +1593,17 @@
       <c r="C21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="21" t="s">
+      <c r="E21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="G21" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -1601,19 +1614,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="3" customFormat="1">
+    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>65</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="9"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="18"/>
       <c r="G24" s="9"/>
-      <c r="I24" s="28"/>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="H24" s="9"/>
+      <c r="J24" s="28"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -1623,14 +1637,14 @@
       <c r="C25" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="24" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>79</v>
       </c>
@@ -1640,11 +1654,11 @@
       <c r="C26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="F26" s="21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>61</v>
       </c>
@@ -1654,11 +1668,11 @@
       <c r="C27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="F27" s="20" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
@@ -1668,28 +1682,28 @@
       <c r="C28" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="F28" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="31" t="s">
+      <c r="F29" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -1699,11 +1713,11 @@
       <c r="C30" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="30" t="s">
+      <c r="F30" s="29" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -1713,12 +1727,12 @@
       <c r="C31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="23"/>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="23"/>
+      <c r="G31" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>14</v>
       </c>
@@ -1728,26 +1742,27 @@
       <c r="C32" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E32" s="30" t="s">
+      <c r="F32" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="3" customFormat="1">
+    <row r="35" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="5"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="17"/>
       <c r="G35" s="5"/>
-      <c r="I35" s="28"/>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="H35" s="5"/>
+      <c r="J35" s="28"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -1757,14 +1772,14 @@
       <c r="C36" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E36" s="20" t="s">
+      <c r="E36" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>11</v>
       </c>
@@ -1774,9 +1789,9 @@
       <c r="C37" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E37" s="23"/>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="F37" s="23"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>16</v>
       </c>
@@ -1787,7 +1802,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>17</v>
       </c>
@@ -1798,19 +1813,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="3" customFormat="1">
+    <row r="41" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="5"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="17"/>
       <c r="G41" s="5"/>
-      <c r="I41" s="28"/>
-    </row>
-    <row r="42" spans="1:9" ht="70">
+      <c r="H41" s="5"/>
+      <c r="J41" s="28"/>
+    </row>
+    <row r="42" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
@@ -1820,17 +1836,17 @@
       <c r="C42" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E42" s="20" t="s">
+      <c r="E42" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F42" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="G42" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>11</v>
       </c>
@@ -1841,19 +1857,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="3" customFormat="1">
+    <row r="45" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="5"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="17"/>
       <c r="G45" s="5"/>
-      <c r="I45" s="28"/>
-    </row>
-    <row r="46" spans="1:9" ht="70">
+      <c r="H45" s="5"/>
+      <c r="J45" s="28"/>
+    </row>
+    <row r="46" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -1863,17 +1880,17 @@
       <c r="C46" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E46" s="26" t="s">
+      <c r="E46" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F46" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="G46" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>11</v>
       </c>
@@ -1884,19 +1901,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="3" customFormat="1">
+    <row r="49" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="5"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="17"/>
       <c r="G49" s="5"/>
-      <c r="I49" s="28"/>
-    </row>
-    <row r="50" spans="1:9" ht="28">
+      <c r="H49" s="5"/>
+      <c r="J49" s="28"/>
+    </row>
+    <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
@@ -1906,17 +1924,17 @@
       <c r="C50" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E50" s="20" t="s">
+      <c r="E50" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F50" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="G50" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>11</v>
       </c>
@@ -1927,19 +1945,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:9" s="3" customFormat="1">
+    <row r="53" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B53" s="9"/>
       <c r="C53" s="14"/>
       <c r="D53" s="14"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="9"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="18"/>
       <c r="G53" s="9"/>
-      <c r="I53" s="28"/>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="H53" s="9"/>
+      <c r="J53" s="28"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -1949,14 +1968,14 @@
       <c r="C54" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E54" s="27" t="s">
+      <c r="E54" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F54" s="27" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>66</v>
       </c>
@@ -1966,11 +1985,11 @@
       <c r="C55" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E55" s="20" t="s">
+      <c r="F55" s="20" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>20</v>
       </c>
@@ -1981,7 +2000,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>21</v>
       </c>
@@ -1992,7 +2011,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>85</v>
       </c>
@@ -2002,23 +2021,24 @@
       <c r="C58" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E58" s="22" t="s">
+      <c r="F58" s="22" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:9" s="3" customFormat="1">
+    <row r="60" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="5"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="17"/>
       <c r="G60" s="5"/>
-      <c r="I60" s="28"/>
-    </row>
-    <row r="61" spans="1:9" ht="56">
+      <c r="H60" s="5"/>
+      <c r="J60" s="28"/>
+    </row>
+    <row r="61" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>0</v>
       </c>
@@ -2028,17 +2048,17 @@
       <c r="C61" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E61" s="22" t="s">
+      <c r="E61" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F61" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="F61" s="4" t="s">
+      <c r="G61" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>11</v>
       </c>
@@ -2049,65 +2069,69 @@
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="3" customFormat="1">
+    <row r="64" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
         <v>24</v>
       </c>
       <c r="B64" s="12"/>
       <c r="C64" s="13"/>
       <c r="D64" s="13"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="12"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="19"/>
       <c r="G64" s="12"/>
-      <c r="I64" s="28"/>
-    </row>
-    <row r="65" spans="1:7">
+      <c r="H64" s="12"/>
+      <c r="J64" s="28"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B65" s="29" t="s">
+      <c r="B65" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C65" s="29"/>
-      <c r="D65" s="29"/>
-      <c r="E65" s="29"/>
-      <c r="F65" s="29"/>
-      <c r="G65" s="29"/>
-    </row>
-    <row r="66" spans="1:7">
+      <c r="C65" s="31"/>
+      <c r="D65" s="31"/>
+      <c r="E65" s="31"/>
+      <c r="F65" s="31"/>
+      <c r="G65" s="31"/>
+      <c r="H65" s="31"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B66" s="29" t="s">
+      <c r="B66" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C66" s="29"/>
-      <c r="D66" s="29"/>
-      <c r="E66" s="29"/>
-      <c r="F66" s="29"/>
-      <c r="G66" s="29"/>
-    </row>
-    <row r="67" spans="1:7">
+      <c r="C66" s="31"/>
+      <c r="D66" s="31"/>
+      <c r="E66" s="31"/>
+      <c r="F66" s="31"/>
+      <c r="G66" s="31"/>
+      <c r="H66" s="31"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B67" s="29" t="s">
+      <c r="B67" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C67" s="29"/>
-      <c r="D67" s="29"/>
-      <c r="E67" s="29"/>
-      <c r="F67" s="29"/>
-      <c r="G67" s="29"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="31"/>
+      <c r="F67" s="31"/>
+      <c r="G67" s="31"/>
+      <c r="H67" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B65:G65"/>
-    <mergeCell ref="B66:G66"/>
-    <mergeCell ref="B67:G67"/>
+    <mergeCell ref="B65:H65"/>
+    <mergeCell ref="B66:H66"/>
+    <mergeCell ref="B67:H67"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;12MdP: Paketshop&amp;C&amp;"-,Fett"&amp;14&amp;UDatenbank-Definition&amp;R&amp;12Seite: &amp;P / &amp;N</oddHeader>
     <oddFooter>&amp;LMichael Ott&amp;RStand 27.11.2011</oddFooter>

</xml_diff>

<commit_message>
Berechtigung + Balsamiq fuer GUI
</commit_message>
<xml_diff>
--- a/additional_files/db/Datenbank_Aufbau_Layout.xlsx
+++ b/additional_files/db/Datenbank_Aufbau_Layout.xlsx
@@ -10,16 +10,11 @@
     <sheet name="Datenbank-Aufbau (Layout)" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="101">
   <si>
     <t>ID</t>
   </si>
@@ -314,6 +309,30 @@
   </si>
   <si>
     <t>Unique</t>
+  </si>
+  <si>
+    <t>&gt; Berechtigung</t>
+  </si>
+  <si>
+    <t>Gruppe = AdressTyp.ID</t>
+  </si>
+  <si>
+    <t>Tabelle</t>
+  </si>
+  <si>
+    <t>TabellenName</t>
+  </si>
+  <si>
+    <t>Feld</t>
+  </si>
+  <si>
+    <t>FeldName</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>z.B. Erfassen-Button</t>
   </si>
 </sst>
 </file>
@@ -825,7 +844,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="52">
+  <cellStyleXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -878,8 +897,18 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -974,8 +1003,33 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="52">
+  <cellStyles count="62">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1007,6 +1061,11 @@
     <cellStyle name="Besuchter Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -1016,6 +1075,11 @@
     <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
@@ -1326,10 +1390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K67"/>
+  <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2124,6 +2188,104 @@
       <c r="G67" s="31"/>
       <c r="H67" s="31"/>
     </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B70" s="35"/>
+      <c r="C70" s="36"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="36"/>
+      <c r="F70" s="38"/>
+      <c r="G70" s="35"/>
+      <c r="H70" s="35"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C71" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D71" s="32"/>
+      <c r="E71" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="F71" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="G71" s="32"/>
+      <c r="H71" s="32"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B72" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C72" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D72" s="32"/>
+      <c r="E72" s="32"/>
+      <c r="F72" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="G72" s="32"/>
+      <c r="H72" s="32"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B73" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C73" s="32"/>
+      <c r="D73" s="32"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="37"/>
+      <c r="G73" s="32"/>
+      <c r="H73" s="33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B74" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C74" s="32"/>
+      <c r="D74" s="32"/>
+      <c r="E74" s="32"/>
+      <c r="F74" s="37"/>
+      <c r="G74" s="32"/>
+      <c r="H74" s="33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="B75" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C75" s="32"/>
+      <c r="D75" s="32"/>
+      <c r="E75" s="32"/>
+      <c r="F75" s="37"/>
+      <c r="G75" s="32"/>
+      <c r="H75" s="33" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B65:H65"/>
@@ -2136,10 +2298,5 @@
     <oddHeader>&amp;L&amp;12MdP: Paketshop&amp;C&amp;"-,Fett"&amp;14&amp;UDatenbank-Definition&amp;R&amp;12Seite: &amp;P / &amp;N</oddHeader>
     <oddFooter>&amp;LMichael Ott&amp;RStand 27.11.2011</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>